<commit_message>
Latest changes and prior settings sensitivity
</commit_message>
<xml_diff>
--- a/Documents/Tables_Models_4.17.24.xlsx
+++ b/Documents/Tables_Models_4.17.24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmenrodriguez/Desktop/Research Projects/BayesBinMix/ecbayesbinmix/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F7212E-2E20-F945-84EB-7A0FD4D16F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7C7FE7-4B47-F34A-807F-1D918DD7878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23000" yWindow="500" windowWidth="14720" windowHeight="20920" firstSheet="6" activeTab="18" xr2:uid="{3C93BFA3-DCF0-6A4C-BE1A-7CEC319431AB}"/>
+    <workbookView xWindow="8280" yWindow="500" windowWidth="19880" windowHeight="17500" firstSheet="5" activeTab="17" xr2:uid="{3C93BFA3-DCF0-6A4C-BE1A-7CEC319431AB}"/>
   </bookViews>
   <sheets>
     <sheet name="old version" sheetId="1" state="hidden" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5570" uniqueCount="3342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5613" uniqueCount="3368">
   <si>
     <t>Not optimal</t>
   </si>
@@ -12136,6 +12136,84 @@
   </si>
   <si>
     <t>Based on defintion from CDC PLACES survey</t>
+  </si>
+  <si>
+    <t>0.750 (0.185)</t>
+  </si>
+  <si>
+    <t>0.781 [0.392, 0.996]</t>
+  </si>
+  <si>
+    <t>0.834 (0.171)</t>
+  </si>
+  <si>
+    <t>0.908 [0.347, 0.997]</t>
+  </si>
+  <si>
+    <t>0.960 (0.119)</t>
+  </si>
+  <si>
+    <t>0.998 [0.182, 1.00]</t>
+  </si>
+  <si>
+    <t>0.787 (0.136)</t>
+  </si>
+  <si>
+    <t>0.789 (0.164)</t>
+  </si>
+  <si>
+    <t>0.892 (0.165)</t>
+  </si>
+  <si>
+    <t>0.866 (0.146)</t>
+  </si>
+  <si>
+    <t>0.815 (0.190)</t>
+  </si>
+  <si>
+    <t>0.812 (0.189)</t>
+  </si>
+  <si>
+    <t>0.614 (0.0849)</t>
+  </si>
+  <si>
+    <t>0.868 (0.176)</t>
+  </si>
+  <si>
+    <t>0.868 (0.154)</t>
+  </si>
+  <si>
+    <t>0.875 (0.172)</t>
+  </si>
+  <si>
+    <t>0.972 [0.352, 0.999]</t>
+  </si>
+  <si>
+    <t>0.943 [0.177, 0.974]</t>
+  </si>
+  <si>
+    <t>0.948 [0.171, 0.999]</t>
+  </si>
+  <si>
+    <t>0.642 [0.350, 0.701]</t>
+  </si>
+  <si>
+    <t>0.887 [0.400, 0.992]</t>
+  </si>
+  <si>
+    <t>0.878 [0.276, 0.992]</t>
+  </si>
+  <si>
+    <t>0.935 [0.503, 0.995]</t>
+  </si>
+  <si>
+    <t>0.980 [0.201, 0.998]</t>
+  </si>
+  <si>
+    <t>0.796 [0.478, 0.989]</t>
+  </si>
+  <si>
+    <t>0.820 [0.385, 0.939]</t>
   </si>
 </sst>
 </file>
@@ -12701,7 +12779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -13120,6 +13198,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -13146,13 +13225,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -13178,10 +13257,16 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13190,26 +13275,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -13223,10 +13293,19 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13549,16 +13628,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="158"/>
+    <col min="1" max="1" width="10.83203125" style="159"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="158"/>
+    <col min="6" max="6" width="10.83203125" style="159"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="17" thickTop="1">
-      <c r="B1" s="156"/>
+      <c r="B1" s="157"/>
       <c r="C1" s="1" t="s">
         <v>240</v>
       </c>
@@ -13570,7 +13649,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" ht="17" thickBot="1">
-      <c r="B2" s="157"/>
+      <c r="B2" s="158"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -16939,10 +17018,10 @@
       <c r="A1" s="31"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
-      <c r="D1" s="172" t="s">
+      <c r="D1" s="173" t="s">
         <v>804</v>
       </c>
-      <c r="E1" s="172"/>
+      <c r="E1" s="173"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="31"/>
@@ -17407,24 +17486,24 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="40"/>
-      <c r="B35" s="173" t="s">
+      <c r="B35" s="174" t="s">
         <v>855</v>
       </c>
-      <c r="C35" s="173"/>
-      <c r="D35" s="173"/>
-      <c r="E35" s="173"/>
-      <c r="F35" s="174" t="s">
+      <c r="C35" s="174"/>
+      <c r="D35" s="174"/>
+      <c r="E35" s="174"/>
+      <c r="F35" s="175" t="s">
         <v>867</v>
       </c>
-      <c r="G35" s="174"/>
-      <c r="H35" s="174"/>
-      <c r="I35" s="174"/>
-      <c r="J35" s="174" t="s">
+      <c r="G35" s="175"/>
+      <c r="H35" s="175"/>
+      <c r="I35" s="175"/>
+      <c r="J35" s="175" t="s">
         <v>868</v>
       </c>
-      <c r="K35" s="174"/>
-      <c r="L35" s="174"/>
-      <c r="M35" s="174"/>
+      <c r="K35" s="175"/>
+      <c r="L35" s="175"/>
+      <c r="M35" s="175"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="41"/>
@@ -17827,12 +17906,12 @@
       <c r="M45" s="46"/>
     </row>
     <row r="48" spans="1:13" ht="32" customHeight="1">
-      <c r="A48" s="175" t="s">
+      <c r="A48" s="176" t="s">
         <v>874</v>
       </c>
-      <c r="B48" s="176"/>
-      <c r="C48" s="176"/>
-      <c r="D48" s="177"/>
+      <c r="B48" s="177"/>
+      <c r="C48" s="177"/>
+      <c r="D48" s="178"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="56" t="s">
@@ -17877,12 +17956,12 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="32" customHeight="1">
-      <c r="A54" s="171" t="s">
+      <c r="A54" s="172" t="s">
         <v>875</v>
       </c>
-      <c r="B54" s="171"/>
-      <c r="C54" s="171"/>
-      <c r="D54" s="171"/>
+      <c r="B54" s="172"/>
+      <c r="C54" s="172"/>
+      <c r="D54" s="172"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="56" t="s">
@@ -18092,31 +18171,31 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="105"/>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="161" t="s">
         <v>2875</v>
       </c>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160" t="s">
+      <c r="C3" s="161"/>
+      <c r="D3" s="161" t="s">
         <v>2876</v>
       </c>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160" t="s">
+      <c r="E3" s="161"/>
+      <c r="F3" s="161" t="s">
         <v>2877</v>
       </c>
-      <c r="G3" s="160"/>
+      <c r="G3" s="161"/>
       <c r="L3" s="105"/>
-      <c r="M3" s="160" t="s">
+      <c r="M3" s="161" t="s">
         <v>2875</v>
       </c>
-      <c r="N3" s="160"/>
-      <c r="O3" s="160" t="s">
+      <c r="N3" s="161"/>
+      <c r="O3" s="161" t="s">
         <v>2876</v>
       </c>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="160" t="s">
+      <c r="P3" s="161"/>
+      <c r="Q3" s="161" t="s">
         <v>2877</v>
       </c>
-      <c r="R3" s="160"/>
+      <c r="R3" s="161"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="105"/>
@@ -18203,10 +18282,10 @@
       <c r="L6" s="119" t="s">
         <v>2928</v>
       </c>
-      <c r="M6" s="184" t="s">
+      <c r="M6" s="179" t="s">
         <v>2879</v>
       </c>
-      <c r="N6" s="184"/>
+      <c r="N6" s="179"/>
       <c r="O6" s="120"/>
       <c r="P6" s="120"/>
       <c r="Q6" s="120"/>
@@ -18300,8 +18379,8 @@
       <c r="E9" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="F9" s="180"/>
-      <c r="G9" s="181"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="184"/>
       <c r="L9" s="119" t="s">
         <v>2931</v>
       </c>
@@ -18313,8 +18392,8 @@
       </c>
       <c r="O9" s="120"/>
       <c r="P9" s="120"/>
-      <c r="Q9" s="182"/>
-      <c r="R9" s="183"/>
+      <c r="Q9" s="181"/>
+      <c r="R9" s="182"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="117" t="s">
@@ -18356,18 +18435,18 @@
       <c r="A11" s="117" t="s">
         <v>799</v>
       </c>
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178" t="s">
+      <c r="C11" s="185"/>
+      <c r="D11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="E11" s="178"/>
-      <c r="F11" s="178" t="s">
+      <c r="E11" s="185"/>
+      <c r="F11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="185"/>
       <c r="L11" s="101" t="s">
         <v>5</v>
       </c>
@@ -18394,19 +18473,19 @@
       <c r="E12" s="116" t="s">
         <v>2900</v>
       </c>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
       <c r="L12" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="M12" s="162" t="s">
+      <c r="M12" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N12" s="162"/>
-      <c r="O12" s="162" t="s">
+      <c r="N12" s="163"/>
+      <c r="O12" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P12" s="162"/>
+      <c r="P12" s="163"/>
       <c r="Q12" s="59"/>
       <c r="R12" s="59"/>
     </row>
@@ -18456,10 +18535,10 @@
       <c r="C14" s="100" t="s">
         <v>3030</v>
       </c>
-      <c r="D14" s="178"/>
-      <c r="E14" s="178"/>
-      <c r="F14" s="178"/>
-      <c r="G14" s="178"/>
+      <c r="D14" s="185"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
       <c r="L14" s="106" t="s">
         <v>10</v>
       </c>
@@ -18502,14 +18581,14 @@
       <c r="A16" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162" t="s">
+      <c r="C16" s="163"/>
+      <c r="D16" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E16" s="162"/>
+      <c r="E16" s="163"/>
       <c r="F16" s="59"/>
       <c r="G16" s="59"/>
       <c r="L16" s="101" t="s">
@@ -18547,14 +18626,14 @@
       <c r="L17" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="M17" s="162" t="s">
+      <c r="M17" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N17" s="162"/>
-      <c r="O17" s="162" t="s">
+      <c r="N17" s="163"/>
+      <c r="O17" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P17" s="162"/>
+      <c r="P17" s="163"/>
       <c r="Q17" s="59"/>
       <c r="R17" s="59"/>
     </row>
@@ -18654,14 +18733,14 @@
       <c r="A21" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="B21" s="162" t="s">
+      <c r="B21" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="162" t="s">
+      <c r="C21" s="163"/>
+      <c r="D21" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E21" s="162"/>
+      <c r="E21" s="163"/>
       <c r="F21" s="59"/>
       <c r="G21" s="59"/>
       <c r="L21" s="101" t="s">
@@ -18699,14 +18778,14 @@
       <c r="L22" s="106" t="s">
         <v>354</v>
       </c>
-      <c r="M22" s="162" t="s">
+      <c r="M22" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N22" s="162"/>
-      <c r="O22" s="162" t="s">
+      <c r="N22" s="163"/>
+      <c r="O22" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P22" s="162"/>
+      <c r="P22" s="163"/>
       <c r="Q22" s="59"/>
       <c r="R22" s="59"/>
     </row>
@@ -18802,14 +18881,14 @@
       <c r="A26" s="106" t="s">
         <v>354</v>
       </c>
-      <c r="B26" s="162" t="s">
+      <c r="B26" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C26" s="162"/>
-      <c r="D26" s="162" t="s">
+      <c r="C26" s="163"/>
+      <c r="D26" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E26" s="162"/>
+      <c r="E26" s="163"/>
       <c r="F26" s="59"/>
       <c r="G26" s="59"/>
       <c r="L26" s="106" t="s">
@@ -18883,18 +18962,18 @@
       <c r="L28" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="M28" s="179" t="s">
+      <c r="M28" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="N28" s="179"/>
-      <c r="O28" s="179" t="s">
+      <c r="N28" s="180"/>
+      <c r="O28" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="P28" s="179"/>
-      <c r="Q28" s="179" t="s">
+      <c r="P28" s="180"/>
+      <c r="Q28" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="R28" s="179"/>
+      <c r="R28" s="180"/>
     </row>
     <row r="29" spans="1:18" ht="18">
       <c r="A29" s="106" t="s">
@@ -18992,33 +19071,33 @@
       <c r="A32" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="179" t="s">
+      <c r="B32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="C32" s="179"/>
-      <c r="D32" s="179" t="s">
+      <c r="C32" s="180"/>
+      <c r="D32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="E32" s="179"/>
-      <c r="F32" s="179" t="s">
+      <c r="E32" s="180"/>
+      <c r="F32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="G32" s="179"/>
+      <c r="G32" s="180"/>
       <c r="L32" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="M32" s="179" t="s">
+      <c r="M32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="N32" s="179"/>
-      <c r="O32" s="179" t="s">
+      <c r="N32" s="180"/>
+      <c r="O32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="P32" s="179"/>
-      <c r="Q32" s="179" t="s">
+      <c r="P32" s="180"/>
+      <c r="Q32" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="R32" s="179"/>
+      <c r="R32" s="180"/>
     </row>
     <row r="33" spans="1:18" ht="18">
       <c r="A33" s="106" t="s">
@@ -19120,18 +19199,18 @@
       <c r="A36" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179" t="s">
+      <c r="C36" s="180"/>
+      <c r="D36" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="E36" s="179"/>
-      <c r="F36" s="179" t="s">
+      <c r="E36" s="180"/>
+      <c r="F36" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="G36" s="179"/>
+      <c r="G36" s="180"/>
       <c r="L36" s="101" t="s">
         <v>360</v>
       </c>
@@ -19167,14 +19246,14 @@
       <c r="L37" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="M37" s="162" t="s">
+      <c r="M37" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N37" s="162"/>
-      <c r="O37" s="162" t="s">
+      <c r="N37" s="163"/>
+      <c r="O37" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P37" s="162"/>
+      <c r="P37" s="163"/>
       <c r="Q37" s="59"/>
       <c r="R37" s="59"/>
     </row>
@@ -19278,14 +19357,14 @@
       <c r="A41" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="162" t="s">
+      <c r="B41" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C41" s="162"/>
-      <c r="D41" s="162" t="s">
+      <c r="C41" s="163"/>
+      <c r="D41" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E41" s="162"/>
+      <c r="E41" s="163"/>
       <c r="F41" s="59"/>
       <c r="G41" s="59"/>
       <c r="L41" s="107" t="s">
@@ -19378,15 +19457,26 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D14:G14"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
@@ -19400,26 +19490,15 @@
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="O22:P22"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19466,31 +19545,31 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="105"/>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="161" t="s">
         <v>2875</v>
       </c>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160" t="s">
+      <c r="C3" s="161"/>
+      <c r="D3" s="161" t="s">
         <v>2876</v>
       </c>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160" t="s">
+      <c r="E3" s="161"/>
+      <c r="F3" s="161" t="s">
         <v>2877</v>
       </c>
-      <c r="G3" s="160"/>
+      <c r="G3" s="161"/>
       <c r="L3" s="105"/>
-      <c r="M3" s="160" t="s">
+      <c r="M3" s="161" t="s">
         <v>2875</v>
       </c>
-      <c r="N3" s="160"/>
-      <c r="O3" s="160" t="s">
+      <c r="N3" s="161"/>
+      <c r="O3" s="161" t="s">
         <v>2876</v>
       </c>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="160" t="s">
+      <c r="P3" s="161"/>
+      <c r="Q3" s="161" t="s">
         <v>2877</v>
       </c>
-      <c r="R3" s="160"/>
+      <c r="R3" s="161"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="105"/>
@@ -19577,10 +19656,10 @@
       <c r="L6" s="119" t="s">
         <v>2928</v>
       </c>
-      <c r="M6" s="184" t="s">
+      <c r="M6" s="179" t="s">
         <v>2879</v>
       </c>
-      <c r="N6" s="184"/>
+      <c r="N6" s="179"/>
       <c r="O6" s="120"/>
       <c r="P6" s="120"/>
       <c r="Q6" s="120"/>
@@ -19674,8 +19753,8 @@
       <c r="E9" s="116" t="s">
         <v>464</v>
       </c>
-      <c r="F9" s="180"/>
-      <c r="G9" s="181"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="184"/>
       <c r="L9" s="119" t="s">
         <v>2931</v>
       </c>
@@ -19687,8 +19766,8 @@
       </c>
       <c r="O9" s="120"/>
       <c r="P9" s="120"/>
-      <c r="Q9" s="182"/>
-      <c r="R9" s="183"/>
+      <c r="Q9" s="181"/>
+      <c r="R9" s="182"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="117" t="s">
@@ -19730,18 +19809,18 @@
       <c r="A11" s="117" t="s">
         <v>799</v>
       </c>
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178" t="s">
+      <c r="C11" s="185"/>
+      <c r="D11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="E11" s="178"/>
-      <c r="F11" s="178" t="s">
+      <c r="E11" s="185"/>
+      <c r="F11" s="185" t="s">
         <v>2879</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="185"/>
       <c r="L11" s="101" t="s">
         <v>5</v>
       </c>
@@ -19768,19 +19847,19 @@
       <c r="E12" s="116" t="s">
         <v>2900</v>
       </c>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
       <c r="L12" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="M12" s="162" t="s">
+      <c r="M12" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N12" s="162"/>
-      <c r="O12" s="162" t="s">
+      <c r="N12" s="163"/>
+      <c r="O12" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P12" s="162"/>
+      <c r="P12" s="163"/>
       <c r="Q12" s="59"/>
       <c r="R12" s="59"/>
     </row>
@@ -19830,10 +19909,10 @@
       <c r="C14" s="116" t="s">
         <v>2689</v>
       </c>
-      <c r="D14" s="178"/>
-      <c r="E14" s="178"/>
-      <c r="F14" s="178"/>
-      <c r="G14" s="178"/>
+      <c r="D14" s="185"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
       <c r="L14" s="106" t="s">
         <v>10</v>
       </c>
@@ -19876,14 +19955,14 @@
       <c r="A16" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162" t="s">
+      <c r="C16" s="163"/>
+      <c r="D16" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E16" s="162"/>
+      <c r="E16" s="163"/>
       <c r="F16" s="59"/>
       <c r="G16" s="59"/>
       <c r="L16" s="101" t="s">
@@ -19921,14 +20000,14 @@
       <c r="L17" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="M17" s="162" t="s">
+      <c r="M17" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N17" s="162"/>
-      <c r="O17" s="162" t="s">
+      <c r="N17" s="163"/>
+      <c r="O17" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P17" s="162"/>
+      <c r="P17" s="163"/>
       <c r="Q17" s="59"/>
       <c r="R17" s="59"/>
     </row>
@@ -20028,23 +20107,23 @@
       <c r="A21" s="106" t="s">
         <v>343</v>
       </c>
-      <c r="B21" s="162" t="s">
+      <c r="B21" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C21" s="162"/>
-      <c r="D21" s="162" t="s">
+      <c r="C21" s="163"/>
+      <c r="D21" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E21" s="162"/>
+      <c r="E21" s="163"/>
       <c r="F21" s="59"/>
       <c r="G21" s="59"/>
       <c r="L21" s="105">
         <v>2006</v>
       </c>
-      <c r="M21" s="162" t="s">
+      <c r="M21" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N21" s="162"/>
+      <c r="N21" s="163"/>
       <c r="O21" s="59"/>
       <c r="P21" s="59"/>
       <c r="Q21" s="59"/>
@@ -20150,10 +20229,10 @@
       <c r="A25" s="105">
         <v>2006</v>
       </c>
-      <c r="B25" s="162" t="s">
+      <c r="B25" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C25" s="162"/>
+      <c r="C25" s="163"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
@@ -20191,10 +20270,10 @@
       </c>
       <c r="M26" s="59"/>
       <c r="N26" s="59"/>
-      <c r="O26" s="162" t="s">
+      <c r="O26" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P26" s="162"/>
+      <c r="P26" s="163"/>
       <c r="Q26" s="59"/>
       <c r="R26" s="59"/>
     </row>
@@ -20276,10 +20355,10 @@
       </c>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
-      <c r="D30" s="162" t="s">
+      <c r="D30" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E30" s="162"/>
+      <c r="E30" s="163"/>
       <c r="F30" s="59"/>
       <c r="G30" s="59"/>
       <c r="L30" s="105">
@@ -20289,10 +20368,10 @@
       <c r="N30" s="59"/>
       <c r="O30" s="59"/>
       <c r="P30" s="59"/>
-      <c r="Q30" s="162" t="s">
+      <c r="Q30" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="R30" s="162"/>
+      <c r="R30" s="163"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="105">
@@ -20374,21 +20453,21 @@
       <c r="C34" s="59"/>
       <c r="D34" s="59"/>
       <c r="E34" s="59"/>
-      <c r="F34" s="162" t="s">
+      <c r="F34" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="G34" s="162"/>
+      <c r="G34" s="163"/>
       <c r="L34" s="106" t="s">
         <v>354</v>
       </c>
-      <c r="M34" s="162" t="s">
+      <c r="M34" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N34" s="162"/>
-      <c r="O34" s="162" t="s">
+      <c r="N34" s="163"/>
+      <c r="O34" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P34" s="162"/>
+      <c r="P34" s="163"/>
       <c r="Q34" s="59"/>
       <c r="R34" s="59"/>
     </row>
@@ -20476,14 +20555,14 @@
       <c r="A38" s="106" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="162" t="s">
+      <c r="B38" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C38" s="162"/>
-      <c r="D38" s="162" t="s">
+      <c r="C38" s="163"/>
+      <c r="D38" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E38" s="162"/>
+      <c r="E38" s="163"/>
       <c r="F38" s="59"/>
       <c r="G38" s="59"/>
       <c r="L38" s="106" t="s">
@@ -20557,18 +20636,18 @@
       <c r="L40" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="M40" s="179" t="s">
+      <c r="M40" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="N40" s="179"/>
-      <c r="O40" s="179" t="s">
+      <c r="N40" s="180"/>
+      <c r="O40" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="P40" s="179"/>
-      <c r="Q40" s="179" t="s">
+      <c r="P40" s="180"/>
+      <c r="Q40" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="R40" s="179"/>
+      <c r="R40" s="180"/>
     </row>
     <row r="41" spans="1:18" ht="18">
       <c r="A41" s="106" t="s">
@@ -20666,33 +20745,33 @@
       <c r="A44" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="179" t="s">
+      <c r="B44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="C44" s="179"/>
-      <c r="D44" s="179" t="s">
+      <c r="C44" s="180"/>
+      <c r="D44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="E44" s="179"/>
-      <c r="F44" s="179" t="s">
+      <c r="E44" s="180"/>
+      <c r="F44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="G44" s="179"/>
+      <c r="G44" s="180"/>
       <c r="L44" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="M44" s="179" t="s">
+      <c r="M44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="N44" s="179"/>
-      <c r="O44" s="179" t="s">
+      <c r="N44" s="180"/>
+      <c r="O44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="P44" s="179"/>
-      <c r="Q44" s="179" t="s">
+      <c r="P44" s="180"/>
+      <c r="Q44" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="R44" s="179"/>
+      <c r="R44" s="180"/>
     </row>
     <row r="45" spans="1:18" ht="18">
       <c r="A45" s="106" t="s">
@@ -20794,18 +20873,18 @@
       <c r="A48" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="179" t="s">
+      <c r="B48" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="C48" s="179"/>
-      <c r="D48" s="179" t="s">
+      <c r="C48" s="180"/>
+      <c r="D48" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="E48" s="179"/>
-      <c r="F48" s="179" t="s">
+      <c r="E48" s="180"/>
+      <c r="F48" s="180" t="s">
         <v>2879</v>
       </c>
-      <c r="G48" s="179"/>
+      <c r="G48" s="180"/>
       <c r="L48" s="101" t="s">
         <v>360</v>
       </c>
@@ -20841,14 +20920,14 @@
       <c r="L49" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="M49" s="162" t="s">
+      <c r="M49" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="N49" s="162"/>
-      <c r="O49" s="162" t="s">
+      <c r="N49" s="163"/>
+      <c r="O49" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="P49" s="162"/>
+      <c r="P49" s="163"/>
       <c r="Q49" s="59"/>
       <c r="R49" s="59"/>
     </row>
@@ -20952,14 +21031,14 @@
       <c r="A53" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="162" t="s">
+      <c r="B53" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="C53" s="162"/>
-      <c r="D53" s="162" t="s">
+      <c r="C53" s="163"/>
+      <c r="D53" s="163" t="s">
         <v>2879</v>
       </c>
-      <c r="E53" s="162"/>
+      <c r="E53" s="163"/>
       <c r="F53" s="59"/>
       <c r="G53" s="59"/>
       <c r="L53" s="107" t="s">
@@ -21042,6 +21121,41 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="Q44:R44"/>
@@ -21055,41 +21169,6 @@
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="O44:P44"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22029,13 +22108,13 @@
     <row r="36" spans="1:11" ht="19">
       <c r="A36" s="125"/>
       <c r="B36" s="126"/>
-      <c r="C36" s="185" t="s">
+      <c r="C36" s="186" t="s">
         <v>3247</v>
       </c>
-      <c r="D36" s="185"/>
-      <c r="E36" s="185"/>
-      <c r="F36" s="185"/>
-      <c r="G36" s="185"/>
+      <c r="D36" s="186"/>
+      <c r="E36" s="186"/>
+      <c r="F36" s="186"/>
+      <c r="G36" s="186"/>
       <c r="H36" s="125"/>
       <c r="I36" s="127"/>
       <c r="J36" s="127"/>
@@ -22860,17 +22939,17 @@
   <sheetData>
     <row r="3" spans="1:13" ht="17" thickBot="1"/>
     <row r="4" spans="1:13" ht="16" customHeight="1" thickBot="1">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="187" t="s">
         <v>3296</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="191"/>
+      <c r="B4" s="188"/>
+      <c r="C4" s="188"/>
+      <c r="D4" s="188"/>
+      <c r="E4" s="188"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="188"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="189"/>
     </row>
     <row r="5" spans="1:13" ht="17" thickBot="1">
       <c r="A5" s="130" t="s">
@@ -22995,24 +23074,24 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="142"/>
-      <c r="B13" s="192" t="s">
+      <c r="B13" s="190" t="s">
         <v>855</v>
       </c>
-      <c r="C13" s="192"/>
-      <c r="D13" s="192"/>
-      <c r="E13" s="192"/>
-      <c r="F13" s="186" t="s">
+      <c r="C13" s="190"/>
+      <c r="D13" s="190"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="191" t="s">
         <v>867</v>
       </c>
-      <c r="G13" s="186"/>
-      <c r="H13" s="186"/>
-      <c r="I13" s="186"/>
-      <c r="J13" s="186" t="s">
+      <c r="G13" s="191"/>
+      <c r="H13" s="191"/>
+      <c r="I13" s="191"/>
+      <c r="J13" s="191" t="s">
         <v>868</v>
       </c>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="186"/>
+      <c r="K13" s="191"/>
+      <c r="L13" s="191"/>
+      <c r="M13" s="191"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="84"/>
@@ -23409,10 +23488,10 @@
     <row r="27" spans="1:13">
       <c r="A27" s="135"/>
       <c r="B27" s="136"/>
-      <c r="C27" s="187" t="s">
+      <c r="C27" s="192" t="s">
         <v>3289</v>
       </c>
-      <c r="D27" s="187"/>
+      <c r="D27" s="192"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="135"/>
@@ -23812,42 +23891,42 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="188" t="s">
+      <c r="A59" s="193" t="s">
         <v>3293</v>
       </c>
-      <c r="B59" s="188"/>
-      <c r="C59" s="188"/>
-      <c r="D59" s="188"/>
-      <c r="E59" s="188"/>
+      <c r="B59" s="193"/>
+      <c r="C59" s="193"/>
+      <c r="D59" s="193"/>
+      <c r="E59" s="193"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="188" t="s">
+      <c r="A60" s="193" t="s">
         <v>3294</v>
       </c>
-      <c r="B60" s="188"/>
-      <c r="C60" s="188"/>
-      <c r="D60" s="188"/>
-      <c r="E60" s="188"/>
+      <c r="B60" s="193"/>
+      <c r="C60" s="193"/>
+      <c r="D60" s="193"/>
+      <c r="E60" s="193"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="188" t="s">
+      <c r="A61" s="193" t="s">
         <v>3295</v>
       </c>
-      <c r="B61" s="188"/>
-      <c r="C61" s="188"/>
-      <c r="D61" s="188"/>
-      <c r="E61" s="188"/>
+      <c r="B61" s="193"/>
+      <c r="C61" s="193"/>
+      <c r="D61" s="193"/>
+      <c r="E61" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A61:E61"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A61:E61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24460,9 +24539,9 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CF6515-1F3E-3D46-9249-A5499ECF535B}">
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -24477,10 +24556,10 @@
     <row r="2" spans="1:4">
       <c r="A2" s="150"/>
       <c r="B2" s="151"/>
-      <c r="C2" s="193" t="s">
+      <c r="C2" s="194" t="s">
         <v>3302</v>
       </c>
-      <c r="D2" s="193"/>
+      <c r="D2" s="194"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="150"/>
@@ -24684,9 +24763,212 @@
         <v>3320</v>
       </c>
     </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="150"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="194" t="s">
+        <v>3302</v>
+      </c>
+      <c r="D21" s="194"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="150"/>
+      <c r="B22" s="152" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C22" s="152" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="152" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="153" t="s">
+        <v>794</v>
+      </c>
+      <c r="B23" s="154">
+        <v>49</v>
+      </c>
+      <c r="C23" s="195" t="s">
+        <v>3342</v>
+      </c>
+      <c r="D23" s="195" t="s">
+        <v>3343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="153" t="s">
+        <v>795</v>
+      </c>
+      <c r="B24" s="154">
+        <v>70</v>
+      </c>
+      <c r="C24" s="195" t="s">
+        <v>3344</v>
+      </c>
+      <c r="D24" s="195" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="153" t="s">
+        <v>796</v>
+      </c>
+      <c r="B25" s="154">
+        <v>379</v>
+      </c>
+      <c r="C25" s="195" t="s">
+        <v>3346</v>
+      </c>
+      <c r="D25" s="195" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="153" t="s">
+        <v>797</v>
+      </c>
+      <c r="B26" s="154">
+        <v>55</v>
+      </c>
+      <c r="C26" s="195" t="s">
+        <v>3348</v>
+      </c>
+      <c r="D26" s="195" t="s">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="153" t="s">
+        <v>798</v>
+      </c>
+      <c r="B27" s="154">
+        <v>26</v>
+      </c>
+      <c r="C27" s="195" t="s">
+        <v>3349</v>
+      </c>
+      <c r="D27" s="195" t="s">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="153" t="s">
+        <v>799</v>
+      </c>
+      <c r="B28" s="154">
+        <v>91</v>
+      </c>
+      <c r="C28" s="195" t="s">
+        <v>3350</v>
+      </c>
+      <c r="D28" s="195" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="153" t="s">
+        <v>800</v>
+      </c>
+      <c r="B29" s="154">
+        <v>78</v>
+      </c>
+      <c r="C29" s="195" t="s">
+        <v>3351</v>
+      </c>
+      <c r="D29" s="195" t="s">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="153" t="s">
+        <v>801</v>
+      </c>
+      <c r="B30" s="154">
+        <v>130</v>
+      </c>
+      <c r="C30" s="195" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D30" s="195" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="153" t="s">
+        <v>802</v>
+      </c>
+      <c r="B31" s="154">
+        <v>52</v>
+      </c>
+      <c r="C31" s="195" t="s">
+        <v>3353</v>
+      </c>
+      <c r="D31" s="195" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="153" t="s">
+        <v>3303</v>
+      </c>
+      <c r="B32" s="154">
+        <v>68</v>
+      </c>
+      <c r="C32" s="195" t="s">
+        <v>3354</v>
+      </c>
+      <c r="D32" s="195" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="153" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B33" s="154">
+        <v>115</v>
+      </c>
+      <c r="C33" s="195" t="s">
+        <v>3355</v>
+      </c>
+      <c r="D33" s="195" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="153" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B34" s="154">
+        <v>295</v>
+      </c>
+      <c r="C34" s="195" t="s">
+        <v>3356</v>
+      </c>
+      <c r="D34" s="195" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="153" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B35" s="154">
+        <v>70</v>
+      </c>
+      <c r="C35" s="195" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D35" s="195" t="s">
+        <v>3358</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24697,8 +24979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E832A9-7BBF-BF4A-B649-830425C6A94E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24716,7 +24998,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="68">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="159" t="s">
         <v>3334</v>
       </c>
       <c r="B2" s="134" t="s">
@@ -24724,7 +25006,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="158"/>
+      <c r="A3" s="159"/>
       <c r="B3" t="s">
         <v>3336</v>
       </c>
@@ -24738,7 +25020,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="156" t="s">
         <v>3338</v>
       </c>
       <c r="B5" t="s">
@@ -26651,17 +26933,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
       <c r="O1" s="72" t="s">
         <v>3248</v>
       </c>
@@ -26679,7 +26961,7 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>3248</v>
       </c>
       <c r="B2" s="70" t="s">
@@ -26709,7 +26991,7 @@
       <c r="J2" s="70" t="s">
         <v>372</v>
       </c>
-      <c r="K2" s="160" t="s">
+      <c r="K2" s="161" t="s">
         <v>359</v>
       </c>
       <c r="O2" s="72"/>
@@ -26725,7 +27007,7 @@
       <c r="S2" s="74"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="159"/>
+      <c r="A3" s="160"/>
       <c r="B3" s="83" t="s">
         <v>882</v>
       </c>
@@ -26753,7 +27035,7 @@
       <c r="J3" s="83" t="s">
         <v>889</v>
       </c>
-      <c r="K3" s="160"/>
+      <c r="K3" s="161"/>
       <c r="O3" s="77" t="s">
         <v>5</v>
       </c>
@@ -29389,7 +29671,7 @@
       <c r="J66" s="59" t="s">
         <v>1620</v>
       </c>
-      <c r="K66" s="162"/>
+      <c r="K66" s="163"/>
       <c r="O66" s="72" t="s">
         <v>119</v>
       </c>
@@ -29435,7 +29717,7 @@
       <c r="J67" s="59" t="s">
         <v>1628</v>
       </c>
-      <c r="K67" s="162"/>
+      <c r="K67" s="163"/>
       <c r="O67" s="72" t="s">
         <v>123</v>
       </c>
@@ -30094,17 +30376,17 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="85"/>
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
       <c r="P1" s="72"/>
       <c r="Q1" s="87" t="s">
         <v>1044</v>
@@ -30120,7 +30402,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="163"/>
+      <c r="A2" s="164"/>
       <c r="B2" s="82" t="s">
         <v>364</v>
       </c>
@@ -30145,7 +30427,7 @@
       <c r="I2" s="82" t="s">
         <v>371</v>
       </c>
-      <c r="J2" s="164" t="s">
+      <c r="J2" s="165" t="s">
         <v>359</v>
       </c>
       <c r="P2" s="72"/>
@@ -30161,7 +30443,7 @@
       <c r="T2" s="88"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="163"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="83" t="s">
         <v>2671</v>
       </c>
@@ -30186,7 +30468,7 @@
       <c r="I3" s="83" t="s">
         <v>2678</v>
       </c>
-      <c r="J3" s="164"/>
+      <c r="J3" s="165"/>
       <c r="P3" s="77" t="s">
         <v>5</v>
       </c>
@@ -32684,7 +32966,7 @@
         <v>2164</v>
       </c>
       <c r="J66" s="59"/>
-      <c r="K66" s="158"/>
+      <c r="K66" s="159"/>
       <c r="P66" s="72" t="s">
         <v>119</v>
       </c>
@@ -32728,7 +33010,7 @@
         <v>2172</v>
       </c>
       <c r="J67" s="59"/>
-      <c r="K67" s="158"/>
+      <c r="K67" s="159"/>
       <c r="P67" s="72" t="s">
         <v>123</v>
       </c>
@@ -33222,14 +33504,14 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="85"/>
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
       <c r="H1" s="91"/>
       <c r="I1" s="81"/>
       <c r="L1" s="72"/>
@@ -33247,7 +33529,7 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="164" t="s">
         <v>2664</v>
       </c>
       <c r="B2" s="82" t="s">
@@ -33268,7 +33550,7 @@
       <c r="G2" s="82" t="s">
         <v>371</v>
       </c>
-      <c r="H2" s="164" t="s">
+      <c r="H2" s="165" t="s">
         <v>359</v>
       </c>
       <c r="L2" s="72"/>
@@ -33284,7 +33566,7 @@
       <c r="P2" s="88"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="163"/>
+      <c r="A3" s="164"/>
       <c r="B3" s="83" t="s">
         <v>2665</v>
       </c>
@@ -33303,7 +33585,7 @@
       <c r="G3" s="83" t="s">
         <v>2670</v>
       </c>
-      <c r="H3" s="164"/>
+      <c r="H3" s="165"/>
       <c r="L3" s="77" t="s">
         <v>5</v>
       </c>
@@ -35896,26 +36178,26 @@
     </row>
     <row r="2" spans="1:11" s="19" customFormat="1">
       <c r="A2" s="21"/>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="167" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="168"/>
-      <c r="D2" s="167" t="s">
+      <c r="C2" s="167"/>
+      <c r="D2" s="168" t="s">
         <v>378</v>
       </c>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167" t="s">
+      <c r="E2" s="168"/>
+      <c r="F2" s="168" t="s">
         <v>379</v>
       </c>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167" t="s">
+      <c r="G2" s="168"/>
+      <c r="H2" s="168" t="s">
         <v>380</v>
       </c>
-      <c r="I2" s="167"/>
-      <c r="J2" s="168" t="s">
+      <c r="I2" s="168"/>
+      <c r="J2" s="167" t="s">
         <v>381</v>
       </c>
-      <c r="K2" s="168"/>
+      <c r="K2" s="167"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="22"/>
@@ -36803,26 +37085,26 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="25"/>
-      <c r="B46" s="168" t="s">
+      <c r="B46" s="167" t="s">
         <v>377</v>
       </c>
-      <c r="C46" s="168"/>
-      <c r="D46" s="167" t="s">
+      <c r="C46" s="167"/>
+      <c r="D46" s="168" t="s">
         <v>378</v>
       </c>
-      <c r="E46" s="167"/>
-      <c r="F46" s="167" t="s">
+      <c r="E46" s="168"/>
+      <c r="F46" s="168" t="s">
         <v>379</v>
       </c>
-      <c r="G46" s="167"/>
-      <c r="H46" s="167" t="s">
+      <c r="G46" s="168"/>
+      <c r="H46" s="168" t="s">
         <v>380</v>
       </c>
-      <c r="I46" s="167"/>
-      <c r="J46" s="168" t="s">
+      <c r="I46" s="168"/>
+      <c r="J46" s="167" t="s">
         <v>381</v>
       </c>
-      <c r="K46" s="168"/>
+      <c r="K46" s="167"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="22"/>
@@ -37649,26 +37931,26 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="26"/>
-      <c r="B89" s="166" t="s">
+      <c r="B89" s="169" t="s">
         <v>377</v>
       </c>
-      <c r="C89" s="166"/>
-      <c r="D89" s="167" t="s">
+      <c r="C89" s="169"/>
+      <c r="D89" s="168" t="s">
         <v>378</v>
       </c>
-      <c r="E89" s="167"/>
-      <c r="F89" s="167" t="s">
+      <c r="E89" s="168"/>
+      <c r="F89" s="168" t="s">
         <v>379</v>
       </c>
-      <c r="G89" s="167"/>
-      <c r="H89" s="167" t="s">
+      <c r="G89" s="168"/>
+      <c r="H89" s="168" t="s">
         <v>380</v>
       </c>
-      <c r="I89" s="167"/>
-      <c r="J89" s="166" t="s">
+      <c r="I89" s="168"/>
+      <c r="J89" s="169" t="s">
         <v>381</v>
       </c>
-      <c r="K89" s="166"/>
+      <c r="K89" s="169"/>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="27"/>
@@ -38420,21 +38702,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="J89:K89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38685,14 +38967,14 @@
       <c r="C13" s="108" t="s">
         <v>3037</v>
       </c>
-      <c r="D13" s="169"/>
-      <c r="E13" s="169"/>
-      <c r="F13" s="169"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="169"/>
-      <c r="K13" s="169"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="170"/>
+      <c r="G13" s="170"/>
+      <c r="H13" s="170"/>
+      <c r="I13" s="170"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="170"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="100" t="s">
@@ -38704,14 +38986,14 @@
       <c r="C14" s="108" t="s">
         <v>3039</v>
       </c>
-      <c r="D14" s="169"/>
-      <c r="E14" s="169"/>
-      <c r="F14" s="169"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="169"/>
-      <c r="J14" s="169"/>
-      <c r="K14" s="169"/>
+      <c r="D14" s="170"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="170"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="170"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="170"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="100" t="s">
@@ -38799,14 +39081,14 @@
       <c r="C19" s="108" t="s">
         <v>3069</v>
       </c>
-      <c r="D19" s="169"/>
-      <c r="E19" s="169"/>
-      <c r="F19" s="169"/>
-      <c r="G19" s="169"/>
-      <c r="H19" s="169"/>
-      <c r="I19" s="169"/>
-      <c r="J19" s="169"/>
-      <c r="K19" s="169"/>
+      <c r="D19" s="170"/>
+      <c r="E19" s="170"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="170"/>
+      <c r="H19" s="170"/>
+      <c r="I19" s="170"/>
+      <c r="J19" s="170"/>
+      <c r="K19" s="170"/>
     </row>
     <row r="20" spans="1:11" ht="18">
       <c r="A20" s="100" t="s">
@@ -38818,14 +39100,14 @@
       <c r="C20" s="108" t="s">
         <v>3071</v>
       </c>
-      <c r="D20" s="169"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="169"/>
-      <c r="K20" s="169"/>
+      <c r="D20" s="170"/>
+      <c r="E20" s="170"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="170"/>
+      <c r="K20" s="170"/>
     </row>
     <row r="21" spans="1:11" ht="18">
       <c r="A21" s="100" t="s">
@@ -38837,14 +39119,14 @@
       <c r="C21" s="108" t="s">
         <v>3080</v>
       </c>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="169"/>
-      <c r="I21" s="169"/>
-      <c r="J21" s="169"/>
-      <c r="K21" s="169"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="170"/>
+      <c r="H21" s="170"/>
+      <c r="I21" s="170"/>
+      <c r="J21" s="170"/>
+      <c r="K21" s="170"/>
     </row>
     <row r="22" spans="1:11" ht="18">
       <c r="A22" s="100" t="s">
@@ -38856,23 +39138,23 @@
       <c r="C22" s="108" t="s">
         <v>3082</v>
       </c>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="169"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="169"/>
-      <c r="K22" s="169"/>
+      <c r="D22" s="170"/>
+      <c r="E22" s="170"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="170"/>
+      <c r="H22" s="170"/>
+      <c r="I22" s="170"/>
+      <c r="J22" s="170"/>
+      <c r="K22" s="170"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="100" t="s">
         <v>3044</v>
       </c>
-      <c r="B23" s="170">
+      <c r="B23" s="171">
         <v>1.21</v>
       </c>
-      <c r="C23" s="170" t="s">
+      <c r="C23" s="171" t="s">
         <v>3046</v>
       </c>
       <c r="D23" s="100"/>
@@ -38888,50 +39170,50 @@
       <c r="A24" s="100" t="s">
         <v>3045</v>
       </c>
-      <c r="B24" s="170"/>
-      <c r="C24" s="170"/>
-      <c r="D24" s="169"/>
-      <c r="E24" s="169"/>
-      <c r="F24" s="169"/>
-      <c r="G24" s="169"/>
-      <c r="H24" s="169"/>
-      <c r="I24" s="169"/>
-      <c r="J24" s="169"/>
-      <c r="K24" s="169"/>
+      <c r="B24" s="171"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="170"/>
+      <c r="H24" s="170"/>
+      <c r="I24" s="170"/>
+      <c r="J24" s="170"/>
+      <c r="K24" s="170"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="100" t="s">
         <v>3044</v>
       </c>
-      <c r="B25" s="170" t="s">
+      <c r="B25" s="171" t="s">
         <v>3048</v>
       </c>
-      <c r="C25" s="170" t="s">
+      <c r="C25" s="171" t="s">
         <v>3049</v>
       </c>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169"/>
-      <c r="H25" s="169"/>
-      <c r="I25" s="169"/>
-      <c r="J25" s="169"/>
-      <c r="K25" s="169"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="170"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="170"/>
+      <c r="H25" s="170"/>
+      <c r="I25" s="170"/>
+      <c r="J25" s="170"/>
+      <c r="K25" s="170"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="100" t="s">
         <v>3047</v>
       </c>
-      <c r="B26" s="170"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="169"/>
-      <c r="E26" s="169"/>
-      <c r="F26" s="169"/>
-      <c r="G26" s="169"/>
-      <c r="H26" s="169"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="169"/>
-      <c r="K26" s="169"/>
+      <c r="B26" s="171"/>
+      <c r="C26" s="171"/>
+      <c r="D26" s="170"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="170"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="100" t="s">
@@ -38943,150 +39225,150 @@
       <c r="C27" s="108" t="s">
         <v>3051</v>
       </c>
-      <c r="D27" s="169"/>
-      <c r="E27" s="169"/>
-      <c r="F27" s="169"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="169"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="169"/>
-      <c r="K27" s="169"/>
+      <c r="D27" s="170"/>
+      <c r="E27" s="170"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="170"/>
+      <c r="I27" s="170"/>
+      <c r="J27" s="170"/>
+      <c r="K27" s="170"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="100" t="s">
         <v>3052</v>
       </c>
-      <c r="B28" s="170">
+      <c r="B28" s="171">
         <v>1.4930000000000001</v>
       </c>
-      <c r="C28" s="170" t="s">
+      <c r="C28" s="171" t="s">
         <v>3054</v>
       </c>
-      <c r="D28" s="169"/>
-      <c r="E28" s="169"/>
-      <c r="F28" s="169"/>
-      <c r="G28" s="169"/>
-      <c r="H28" s="169"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="169"/>
-      <c r="K28" s="169"/>
+      <c r="D28" s="170"/>
+      <c r="E28" s="170"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="170"/>
+      <c r="I28" s="170"/>
+      <c r="J28" s="170"/>
+      <c r="K28" s="170"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="100" t="s">
         <v>3053</v>
       </c>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="169"/>
-      <c r="F29" s="169"/>
-      <c r="G29" s="169"/>
-      <c r="H29" s="169"/>
-      <c r="I29" s="169"/>
-      <c r="J29" s="169"/>
-      <c r="K29" s="169"/>
+      <c r="B29" s="171"/>
+      <c r="C29" s="171"/>
+      <c r="D29" s="170"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="170"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="170"/>
+      <c r="K29" s="170"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B30" s="170" t="s">
+      <c r="B30" s="171" t="s">
         <v>3057</v>
       </c>
-      <c r="C30" s="170" t="s">
+      <c r="C30" s="171" t="s">
         <v>3058</v>
       </c>
-      <c r="D30" s="169"/>
-      <c r="E30" s="169"/>
-      <c r="F30" s="169"/>
-      <c r="G30" s="169"/>
-      <c r="H30" s="169"/>
-      <c r="I30" s="169"/>
-      <c r="J30" s="169"/>
-      <c r="K30" s="169"/>
+      <c r="D30" s="170"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="170"/>
+      <c r="H30" s="170"/>
+      <c r="I30" s="170"/>
+      <c r="J30" s="170"/>
+      <c r="K30" s="170"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="100" t="s">
         <v>3056</v>
       </c>
-      <c r="B31" s="170"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="169"/>
+      <c r="B31" s="171"/>
+      <c r="C31" s="171"/>
+      <c r="D31" s="170"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="170"/>
+      <c r="I31" s="170"/>
+      <c r="J31" s="170"/>
+      <c r="K31" s="170"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B32" s="170">
+      <c r="B32" s="171">
         <v>1.9430000000000001</v>
       </c>
-      <c r="C32" s="170" t="s">
+      <c r="C32" s="171" t="s">
         <v>3061</v>
       </c>
-      <c r="D32" s="169"/>
-      <c r="E32" s="169"/>
-      <c r="F32" s="169"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="169"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="169"/>
-      <c r="K32" s="169"/>
+      <c r="D32" s="170"/>
+      <c r="E32" s="170"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="170"/>
+      <c r="H32" s="170"/>
+      <c r="I32" s="170"/>
+      <c r="J32" s="170"/>
+      <c r="K32" s="170"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="100" t="s">
         <v>3059</v>
       </c>
-      <c r="B33" s="170"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="169"/>
-      <c r="K33" s="169"/>
+      <c r="B33" s="171"/>
+      <c r="C33" s="171"/>
+      <c r="D33" s="170"/>
+      <c r="E33" s="170"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="170"/>
+      <c r="I33" s="170"/>
+      <c r="J33" s="170"/>
+      <c r="K33" s="170"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B34" s="170">
+      <c r="B34" s="171">
         <v>1.089</v>
       </c>
-      <c r="C34" s="170" t="s">
+      <c r="C34" s="171" t="s">
         <v>3063</v>
       </c>
-      <c r="D34" s="169"/>
-      <c r="E34" s="169"/>
-      <c r="F34" s="169"/>
-      <c r="G34" s="169"/>
-      <c r="H34" s="169"/>
-      <c r="I34" s="169"/>
-      <c r="J34" s="169"/>
-      <c r="K34" s="169"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="170"/>
+      <c r="F34" s="170"/>
+      <c r="G34" s="170"/>
+      <c r="H34" s="170"/>
+      <c r="I34" s="170"/>
+      <c r="J34" s="170"/>
+      <c r="K34" s="170"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="100" t="s">
         <v>3062</v>
       </c>
-      <c r="B35" s="170"/>
-      <c r="C35" s="170"/>
-      <c r="D35" s="169"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="169"/>
-      <c r="G35" s="169"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="169"/>
-      <c r="K35" s="169"/>
+      <c r="B35" s="171"/>
+      <c r="C35" s="171"/>
+      <c r="D35" s="170"/>
+      <c r="E35" s="170"/>
+      <c r="F35" s="170"/>
+      <c r="G35" s="170"/>
+      <c r="H35" s="170"/>
+      <c r="I35" s="170"/>
+      <c r="J35" s="170"/>
+      <c r="K35" s="170"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="100" t="s">
@@ -39095,14 +39377,14 @@
       <c r="B36" s="108">
         <v>3749</v>
       </c>
-      <c r="D36" s="169"/>
-      <c r="E36" s="169"/>
-      <c r="F36" s="169"/>
-      <c r="G36" s="169"/>
-      <c r="H36" s="169"/>
-      <c r="I36" s="169"/>
-      <c r="J36" s="169"/>
-      <c r="K36" s="169"/>
+      <c r="D36" s="170"/>
+      <c r="E36" s="170"/>
+      <c r="F36" s="170"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="170"/>
+      <c r="I36" s="170"/>
+      <c r="J36" s="170"/>
+      <c r="K36" s="170"/>
     </row>
     <row r="37" spans="1:11" ht="18">
       <c r="A37" s="100" t="s">
@@ -39111,27 +39393,27 @@
       <c r="B37" s="108">
         <v>0.125</v>
       </c>
-      <c r="D37" s="169"/>
-      <c r="E37" s="169"/>
-      <c r="F37" s="169"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="169"/>
-      <c r="I37" s="169"/>
-      <c r="J37" s="169"/>
-      <c r="K37" s="169"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="170"/>
+      <c r="I37" s="170"/>
+      <c r="J37" s="170"/>
+      <c r="K37" s="170"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="99" t="s">
         <v>489</v>
       </c>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
-      <c r="F38" s="169"/>
-      <c r="G38" s="169"/>
-      <c r="H38" s="169"/>
-      <c r="I38" s="169"/>
-      <c r="J38" s="169"/>
-      <c r="K38" s="169"/>
+      <c r="D38" s="170"/>
+      <c r="E38" s="170"/>
+      <c r="F38" s="170"/>
+      <c r="G38" s="170"/>
+      <c r="H38" s="170"/>
+      <c r="I38" s="170"/>
+      <c r="J38" s="170"/>
+      <c r="K38" s="170"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="100"/>
@@ -39241,10 +39523,10 @@
       <c r="A49" s="100" t="s">
         <v>3033</v>
       </c>
-      <c r="B49" s="169">
+      <c r="B49" s="170">
         <v>0.61599999999999999</v>
       </c>
-      <c r="C49" s="169" t="s">
+      <c r="C49" s="170" t="s">
         <v>3088</v>
       </c>
       <c r="D49" s="100"/>
@@ -39254,8 +39536,8 @@
       <c r="A50" s="100" t="s">
         <v>3034</v>
       </c>
-      <c r="B50" s="169"/>
-      <c r="C50" s="169"/>
+      <c r="B50" s="170"/>
+      <c r="C50" s="170"/>
       <c r="D50" s="100"/>
       <c r="E50" s="100"/>
     </row>
@@ -39263,10 +39545,10 @@
       <c r="A51" s="100" t="s">
         <v>3033</v>
       </c>
-      <c r="B51" s="169">
+      <c r="B51" s="170">
         <v>1.1279999999999999</v>
       </c>
-      <c r="C51" s="169" t="s">
+      <c r="C51" s="170" t="s">
         <v>3089</v>
       </c>
       <c r="D51" s="100"/>
@@ -39276,10 +39558,10 @@
       <c r="A52" s="100" t="s">
         <v>3036</v>
       </c>
-      <c r="B52" s="169"/>
-      <c r="C52" s="169"/>
-      <c r="D52" s="169"/>
-      <c r="E52" s="169"/>
+      <c r="B52" s="170"/>
+      <c r="C52" s="170"/>
+      <c r="D52" s="170"/>
+      <c r="E52" s="170"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="100" t="s">
@@ -39291,8 +39573,8 @@
       <c r="C53" s="100" t="s">
         <v>3090</v>
       </c>
-      <c r="D53" s="169"/>
-      <c r="E53" s="169"/>
+      <c r="D53" s="170"/>
+      <c r="E53" s="170"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="100" t="s">
@@ -39304,8 +39586,8 @@
       <c r="C54" s="100" t="s">
         <v>3091</v>
       </c>
-      <c r="D54" s="169"/>
-      <c r="E54" s="169"/>
+      <c r="D54" s="170"/>
+      <c r="E54" s="170"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="100" t="s">
@@ -39317,8 +39599,8 @@
       <c r="C55" s="100" t="s">
         <v>3092</v>
       </c>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
+      <c r="D55" s="170"/>
+      <c r="E55" s="170"/>
     </row>
     <row r="56" spans="1:5" ht="18">
       <c r="A56" s="100" t="s">
@@ -39402,10 +39684,10 @@
       <c r="A62" s="100" t="s">
         <v>3044</v>
       </c>
-      <c r="B62" s="169">
+      <c r="B62" s="170">
         <v>1.1850000000000001</v>
       </c>
-      <c r="C62" s="169" t="s">
+      <c r="C62" s="170" t="s">
         <v>3105</v>
       </c>
       <c r="D62" s="100"/>
@@ -39415,8 +39697,8 @@
       <c r="A63" s="100" t="s">
         <v>3045</v>
       </c>
-      <c r="B63" s="169"/>
-      <c r="C63" s="169"/>
+      <c r="B63" s="170"/>
+      <c r="C63" s="170"/>
       <c r="D63" s="100"/>
       <c r="E63" s="100"/>
     </row>
@@ -39424,10 +39706,10 @@
       <c r="A64" s="100" t="s">
         <v>3044</v>
       </c>
-      <c r="B64" s="169" t="s">
+      <c r="B64" s="170" t="s">
         <v>3106</v>
       </c>
-      <c r="C64" s="169" t="s">
+      <c r="C64" s="170" t="s">
         <v>3107</v>
       </c>
       <c r="D64" s="100"/>
@@ -39437,10 +39719,10 @@
       <c r="A65" s="100" t="s">
         <v>3047</v>
       </c>
-      <c r="B65" s="169"/>
-      <c r="C65" s="169"/>
-      <c r="D65" s="169"/>
-      <c r="E65" s="169"/>
+      <c r="B65" s="170"/>
+      <c r="C65" s="170"/>
+      <c r="D65" s="170"/>
+      <c r="E65" s="170"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="100" t="s">
@@ -39452,39 +39734,39 @@
       <c r="C66" s="100" t="s">
         <v>3108</v>
       </c>
-      <c r="D66" s="169"/>
-      <c r="E66" s="169"/>
+      <c r="D66" s="170"/>
+      <c r="E66" s="170"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="100" t="s">
         <v>3052</v>
       </c>
-      <c r="B67" s="169">
+      <c r="B67" s="170">
         <v>1.484</v>
       </c>
-      <c r="C67" s="169" t="s">
+      <c r="C67" s="170" t="s">
         <v>3109</v>
       </c>
-      <c r="D67" s="169"/>
-      <c r="E67" s="169"/>
+      <c r="D67" s="170"/>
+      <c r="E67" s="170"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="100" t="s">
         <v>3053</v>
       </c>
-      <c r="B68" s="169"/>
-      <c r="C68" s="169"/>
-      <c r="D68" s="169"/>
-      <c r="E68" s="169"/>
+      <c r="B68" s="170"/>
+      <c r="C68" s="170"/>
+      <c r="D68" s="170"/>
+      <c r="E68" s="170"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B69" s="169" t="s">
+      <c r="B69" s="170" t="s">
         <v>3110</v>
       </c>
-      <c r="C69" s="169" t="s">
+      <c r="C69" s="170" t="s">
         <v>3111</v>
       </c>
       <c r="D69" s="100"/>
@@ -39494,54 +39776,54 @@
       <c r="A70" s="100" t="s">
         <v>3056</v>
       </c>
-      <c r="B70" s="169"/>
-      <c r="C70" s="169"/>
-      <c r="D70" s="169"/>
-      <c r="E70" s="169"/>
+      <c r="B70" s="170"/>
+      <c r="C70" s="170"/>
+      <c r="D70" s="170"/>
+      <c r="E70" s="170"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B71" s="169" t="s">
+      <c r="B71" s="170" t="s">
         <v>3112</v>
       </c>
-      <c r="C71" s="169" t="s">
+      <c r="C71" s="170" t="s">
         <v>3113</v>
       </c>
-      <c r="D71" s="169"/>
-      <c r="E71" s="169"/>
+      <c r="D71" s="170"/>
+      <c r="E71" s="170"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="100" t="s">
         <v>3059</v>
       </c>
-      <c r="B72" s="169"/>
-      <c r="C72" s="169"/>
-      <c r="D72" s="169"/>
-      <c r="E72" s="169"/>
+      <c r="B72" s="170"/>
+      <c r="C72" s="170"/>
+      <c r="D72" s="170"/>
+      <c r="E72" s="170"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="100" t="s">
         <v>3055</v>
       </c>
-      <c r="B73" s="169">
+      <c r="B73" s="170">
         <v>1.0760000000000001</v>
       </c>
-      <c r="C73" s="169" t="s">
+      <c r="C73" s="170" t="s">
         <v>3114</v>
       </c>
-      <c r="D73" s="169"/>
-      <c r="E73" s="169"/>
+      <c r="D73" s="170"/>
+      <c r="E73" s="170"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="100" t="s">
         <v>3062</v>
       </c>
-      <c r="B74" s="169"/>
-      <c r="C74" s="169"/>
-      <c r="D74" s="169"/>
-      <c r="E74" s="169"/>
+      <c r="B74" s="170"/>
+      <c r="C74" s="170"/>
+      <c r="D74" s="170"/>
+      <c r="E74" s="170"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="100" t="s">
@@ -39551,8 +39833,8 @@
         <v>3749</v>
       </c>
       <c r="C75"/>
-      <c r="D75" s="169"/>
-      <c r="E75" s="169"/>
+      <c r="D75" s="170"/>
+      <c r="E75" s="170"/>
     </row>
     <row r="76" spans="1:5" ht="18">
       <c r="A76" s="100" t="s">
@@ -39572,11 +39854,83 @@
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="H30:H38"/>
+    <mergeCell ref="I30:I38"/>
+    <mergeCell ref="J30:J38"/>
+    <mergeCell ref="K30:K38"/>
+    <mergeCell ref="D30:D38"/>
+    <mergeCell ref="E30:E38"/>
+    <mergeCell ref="F30:F38"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="G30:G38"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D74:D75"/>
     <mergeCell ref="E74:E75"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:C29"/>
@@ -39593,83 +39947,11 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="G30:G38"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="D30:D38"/>
-    <mergeCell ref="E30:E38"/>
-    <mergeCell ref="F30:F38"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="H30:H38"/>
-    <mergeCell ref="I30:I38"/>
-    <mergeCell ref="J30:J38"/>
-    <mergeCell ref="K30:K38"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>